<commit_message>
This is my extensive learning of transitioning to Flask. I have figured out how to move variables from one place to another and I think it will be easier for this portion of the website.
</commit_message>
<xml_diff>
--- a/docs/Book1.xlsx
+++ b/docs/Book1.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/delimam_uoguelph_ca/Documents/Robotics Stuff/ugrt.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{E5A30729-A1C8-485A-8195-861A4AC2388B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2690C664-8F8A-49EA-80DB-EC501BA02F1B}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{E5A30729-A1C8-485A-8195-861A4AC2388B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4FBE58B-1D2E-415A-9EEB-F52D6B301C06}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
+    <workbookView xWindow="7185" yWindow="2880" windowWidth="21600" windowHeight="11175" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,56 +36,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>create</t>
-  </si>
-  <si>
-    <t>craft</t>
-  </si>
-  <si>
-    <t>what</t>
-  </si>
-  <si>
-    <t>is</t>
-  </si>
-  <si>
-    <t>the</t>
-  </si>
-  <si>
-    <t>Correct Ammount</t>
-  </si>
-  <si>
-    <t>This</t>
-  </si>
-  <si>
-    <t>row</t>
-  </si>
-  <si>
-    <t>two</t>
-  </si>
-  <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">this </t>
-  </si>
-  <si>
-    <t xml:space="preserve">is </t>
-  </si>
-  <si>
-    <t xml:space="preserve">going </t>
-  </si>
-  <si>
-    <t>well</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -133,6 +86,91 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Title</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>little title</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>Little Blurb</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>BIG BLURB</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Impressive Number #1</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Electrical</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>electrical</v>
+          </cell>
+          <cell r="C2" t="str">
+            <v>The electrical team is responsible for creating the electrical system of the rover and interfacing it with the mechanical and programming teams</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>Big blurb for electrical</v>
+          </cell>
+          <cell r="E2" t="str">
+            <v>6000m</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Mechanical</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>mechanical</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>The mechanical team is responsible for creating the chassis of the rover as well as coordinating all the moving components.</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>bigger blurb for mech</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>233kg</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Business</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>business</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>The business teams is required to create all the information we have available on the website. They go out and find sponsors as well as coordonate and manage our social medias.</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v>decent sized blurb for business</v>
+          </cell>
+          <cell r="E4" t="str">
+            <v>24550 posts</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -455,65 +493,97 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="A1" t="str">
+        <f>[1]Sheet1!A1</f>
+        <v>Title</v>
+      </c>
+      <c r="B1" t="str">
+        <f>[1]Sheet1!B1</f>
+        <v>little title</v>
+      </c>
+      <c r="C1" t="str">
+        <f>[1]Sheet1!C1</f>
+        <v>Little Blurb</v>
+      </c>
+      <c r="D1" t="str">
+        <f>[1]Sheet1!D1</f>
+        <v>BIG BLURB</v>
+      </c>
+      <c r="E1" t="str">
+        <f>[1]Sheet1!E1</f>
+        <v>Impressive Number #1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
+      <c r="A2" t="str">
+        <f>[1]Sheet1!A2</f>
+        <v>Electrical</v>
+      </c>
+      <c r="B2" t="str">
+        <f>[1]Sheet1!B2</f>
+        <v>electrical</v>
+      </c>
+      <c r="C2" t="str">
+        <f>[1]Sheet1!C2</f>
+        <v>The electrical team is responsible for creating the electrical system of the rover and interfacing it with the mechanical and programming teams</v>
+      </c>
+      <c r="D2" t="str">
+        <f>[1]Sheet1!D2</f>
+        <v>Big blurb for electrical</v>
+      </c>
+      <c r="E2" t="str">
+        <f>[1]Sheet1!E2</f>
+        <v>6000m</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
+      <c r="A3" t="str">
+        <f>[1]Sheet1!A3</f>
+        <v>Mechanical</v>
+      </c>
+      <c r="B3" t="str">
+        <f>[1]Sheet1!B3</f>
+        <v>mechanical</v>
+      </c>
+      <c r="C3" t="str">
+        <f>[1]Sheet1!C3</f>
+        <v>The mechanical team is responsible for creating the chassis of the rover as well as coordinating all the moving components.</v>
+      </c>
+      <c r="D3" t="str">
+        <f>[1]Sheet1!D3</f>
+        <v>bigger blurb for mech</v>
+      </c>
+      <c r="E3" t="str">
+        <f>[1]Sheet1!E3</f>
+        <v>233kg</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+      <c r="A4" t="str">
+        <f>[1]Sheet1!A4</f>
+        <v>Business</v>
+      </c>
+      <c r="B4" t="str">
+        <f>[1]Sheet1!B4</f>
+        <v>business</v>
+      </c>
+      <c r="C4" t="str">
+        <f>[1]Sheet1!C4</f>
+        <v>The business teams is required to create all the information we have available on the website. They go out and find sponsors as well as coordonate and manage our social medias.</v>
+      </c>
+      <c r="D4" t="str">
+        <f>[1]Sheet1!D4</f>
+        <v>decent sized blurb for business</v>
+      </c>
+      <c r="E4" t="str">
+        <f>[1]Sheet1!E4</f>
+        <v>24550 posts</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This is an update. I've been refining the layout and playing with pulling images in from locations. That might be something we hard code in because you'll have to access the code anyway. I'm also interested in shifting from an excel sheet to a database.
</commit_message>
<xml_diff>
--- a/docs/Book1.xlsx
+++ b/docs/Book1.xlsx
@@ -5,19 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/delimam_uoguelph_ca/Documents/Robotics Stuff/ugrt.github.io/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markd\OneDrive - University of Guelph\Robotics Stuff\ugrt.github.io\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{E5A30729-A1C8-485A-8195-861A4AC2388B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4FBE58B-1D2E-415A-9EEB-F52D6B301C06}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C81EEF6-CB5B-47D7-A416-2756DAEBB15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="2880" windowWidth="21600" windowHeight="11175" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
+    <workbookView xWindow="11110" yWindow="0" windowWidth="11380" windowHeight="13370" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,6 +33,77 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>little title</t>
+  </si>
+  <si>
+    <t>Little Blurb</t>
+  </si>
+  <si>
+    <t>BIG BLURB</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>electrical</t>
+  </si>
+  <si>
+    <t>The electrical team is responsible for creating the electrical system of the rover and interfacing it with the mechanical and programming teams</t>
+  </si>
+  <si>
+    <t>Big blurb for electrical</t>
+  </si>
+  <si>
+    <t>Mechanical</t>
+  </si>
+  <si>
+    <t>mechanical</t>
+  </si>
+  <si>
+    <t>The mechanical team is responsible for creating the chassis of the rover as well as coordinating all the moving components.</t>
+  </si>
+  <si>
+    <t>bigger blurb for mech</t>
+  </si>
+  <si>
+    <t>decent sized blurb for business</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+  <si>
+    <t>programming</t>
+  </si>
+  <si>
+    <t>craxy, no?</t>
+  </si>
+  <si>
+    <t>Lets see if me updating this changes the shit…</t>
+  </si>
+  <si>
+    <t>Image path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url_for('static',filename='it in the hall.jpg') </t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>marketing</t>
+  </si>
+  <si>
+    <t>The marketing team is required to create all the information we have available on the website. They go out and find sponsors as well as coordonate and manage our social medias.</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69,8 +137,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -86,91 +157,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Title</v>
-          </cell>
-          <cell r="B1" t="str">
-            <v>little title</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>Little Blurb</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>BIG BLURB</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>Impressive Number #1</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Electrical</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>electrical</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>The electrical team is responsible for creating the electrical system of the rover and interfacing it with the mechanical and programming teams</v>
-          </cell>
-          <cell r="D2" t="str">
-            <v>Big blurb for electrical</v>
-          </cell>
-          <cell r="E2" t="str">
-            <v>6000m</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Mechanical</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>mechanical</v>
-          </cell>
-          <cell r="C3" t="str">
-            <v>The mechanical team is responsible for creating the chassis of the rover as well as coordinating all the moving components.</v>
-          </cell>
-          <cell r="D3" t="str">
-            <v>bigger blurb for mech</v>
-          </cell>
-          <cell r="E3" t="str">
-            <v>233kg</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Business</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>business</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>The business teams is required to create all the information we have available on the website. They go out and find sponsors as well as coordonate and manage our social medias.</v>
-          </cell>
-          <cell r="D4" t="str">
-            <v>decent sized blurb for business</v>
-          </cell>
-          <cell r="E4" t="str">
-            <v>24550 posts</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -490,103 +476,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2CFC88-1D52-4579-843F-FBBB9CB93435}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="26" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="str">
-        <f>[1]Sheet1!A1</f>
-        <v>Title</v>
-      </c>
-      <c r="B1" t="str">
-        <f>[1]Sheet1!B1</f>
-        <v>little title</v>
-      </c>
-      <c r="C1" t="str">
-        <f>[1]Sheet1!C1</f>
-        <v>Little Blurb</v>
-      </c>
-      <c r="D1" t="str">
-        <f>[1]Sheet1!D1</f>
-        <v>BIG BLURB</v>
-      </c>
-      <c r="E1" t="str">
-        <f>[1]Sheet1!E1</f>
-        <v>Impressive Number #1</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f>[1]Sheet1!A2</f>
-        <v>Electrical</v>
-      </c>
-      <c r="B2" t="str">
-        <f>[1]Sheet1!B2</f>
-        <v>electrical</v>
-      </c>
-      <c r="C2" t="str">
-        <f>[1]Sheet1!C2</f>
-        <v>The electrical team is responsible for creating the electrical system of the rover and interfacing it with the mechanical and programming teams</v>
-      </c>
-      <c r="D2" t="str">
-        <f>[1]Sheet1!D2</f>
-        <v>Big blurb for electrical</v>
-      </c>
-      <c r="E2" t="str">
-        <f>[1]Sheet1!E2</f>
-        <v>6000m</v>
+    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f>[1]Sheet1!A3</f>
-        <v>Mechanical</v>
-      </c>
-      <c r="B3" t="str">
-        <f>[1]Sheet1!B3</f>
-        <v>mechanical</v>
-      </c>
-      <c r="C3" t="str">
-        <f>[1]Sheet1!C3</f>
-        <v>The mechanical team is responsible for creating the chassis of the rover as well as coordinating all the moving components.</v>
-      </c>
-      <c r="D3" t="str">
-        <f>[1]Sheet1!D3</f>
-        <v>bigger blurb for mech</v>
-      </c>
-      <c r="E3" t="str">
-        <f>[1]Sheet1!E3</f>
-        <v>233kg</v>
+    <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f>[1]Sheet1!A4</f>
-        <v>Business</v>
-      </c>
-      <c r="B4" t="str">
-        <f>[1]Sheet1!B4</f>
-        <v>business</v>
-      </c>
-      <c r="C4" t="str">
-        <f>[1]Sheet1!C4</f>
-        <v>The business teams is required to create all the information we have available on the website. They go out and find sponsors as well as coordonate and manage our social medias.</v>
-      </c>
-      <c r="D4" t="str">
-        <f>[1]Sheet1!D4</f>
-        <v>decent sized blurb for business</v>
-      </c>
-      <c r="E4" t="str">
-        <f>[1]Sheet1!E4</f>
-        <v>24550 posts</v>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>